<commit_message>
ajuste casos de testes
</commit_message>
<xml_diff>
--- a/Casos de testes/Casos de testes.xlsx
+++ b/Casos de testes/Casos de testes.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Exemplo\portfolio\Casos de testes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0B4B99-D3B3-4D2A-8CBB-6E53F6EDDAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Requisito" sheetId="1" r:id="rId1"/>
+    <sheet name="Cenários" sheetId="2" r:id="rId2"/>
+    <sheet name="Casos de testes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +26,30 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>TELA DE CADASTRO DE CLIENTE</t>
+  </si>
+  <si>
+    <t>NECESSITO DE UMA TELA DE CADASTRO DE CLIENTE COM A POSSIBILIDADE DE:
+-CONSULTAR E APRESENTAR O RESULTADO EM FORMA DE LISTA
+-CADASTRAR UM NOVO CLIENTE EM OUTRA TELA
+-EDITAR E VISUALIZAR EM OUTRA TELA
+-EXCLUIR A PARTIR DA LISTA
+-PAGINAR A LISTA
+-EXPORTAR OS DADOS PARA PLANILHA EXCEL
+-IMPRIMIR A LISTA E O CLIENTE</t>
+  </si>
+  <si>
+    <t>REQUISITOS</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +57,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -45,12 +88,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -66,6 +185,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>221527</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>23213</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF8B69BF-26DB-B655-2499-8EE1FA8C88A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6713220" y="335280"/>
+          <a:ext cx="6309907" cy="4077053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +498,400 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="8"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="8"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="8"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="8"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="B17:J22"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:J28"/>
+    <mergeCell ref="A2:J9"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="B11:J16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEA7017-2B0D-4810-92A9-2626391EACBF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0F5F09-2DFF-4109-9612-C1E81C19757D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>